<commit_message>
Updates for 2024 elementary school notices
</commit_message>
<xml_diff>
--- a/vaccine_reference.xlsx
+++ b/vaccine_reference.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B4EF38-ABFA-49D1-947F-453C7B2D73AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D8B3F2-455B-4FF7-99DA-44CACB396AB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{2E6AD201-1276-4977-81B0-F9687B5204AE}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="115">
   <si>
     <t>Diphtheria</t>
   </si>
@@ -351,6 +351,15 @@
   </si>
   <si>
     <t>Men-C-A</t>
+  </si>
+  <si>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>Hib-HB</t>
+  </si>
+  <si>
+    <t>Inf High Dose (TIV)</t>
   </si>
 </sst>
 </file>
@@ -1366,9 +1375,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25DCE65C-B951-4D95-B8AA-F65727F774E0}" name="Table1" displayName="Table1" ref="A1:P98" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P98">
-    <sortCondition ref="A1:A98"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{25DCE65C-B951-4D95-B8AA-F65727F774E0}" name="Table1" displayName="Table1" ref="A1:P101" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P101">
+    <sortCondition ref="A1:A101"/>
   </sortState>
   <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{9672583D-60D1-417D-9B52-68046C0762EF}" name="Vaccine" dataDxfId="15"/>
@@ -1709,11 +1718,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CDF4E00-411E-4C73-B8B9-C868A5AAFE62}">
-  <dimension ref="A1:P98"/>
+  <dimension ref="A1:P101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S52" sqref="S52"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46:P46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1874,7 +1883,7 @@
     </row>
     <row r="4" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="B4" s="5">
         <v>0</v>
@@ -1924,7 +1933,7 @@
     </row>
     <row r="5" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="B5" s="5">
         <v>0</v>
@@ -1974,7 +1983,7 @@
     </row>
     <row r="6" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" s="5">
         <v>0</v>
@@ -2024,66 +2033,66 @@
     </row>
     <row r="7" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="5">
+        <v>0</v>
+      </c>
+      <c r="P7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
-        <v>0</v>
-      </c>
-      <c r="K7" s="5">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5">
-        <v>0</v>
-      </c>
-      <c r="M7" s="5">
-        <v>0</v>
-      </c>
-      <c r="N7" s="5">
-        <v>0</v>
-      </c>
-      <c r="O7" s="5">
-        <v>0</v>
-      </c>
-      <c r="P7" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
       <c r="C8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
@@ -2124,7 +2133,7 @@
     </row>
     <row r="9" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
@@ -2154,7 +2163,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="5">
         <v>0</v>
@@ -2174,7 +2183,7 @@
     </row>
     <row r="10" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
@@ -2210,7 +2219,7 @@
         <v>0</v>
       </c>
       <c r="M10" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="5">
         <v>0</v>
@@ -2224,7 +2233,7 @@
     </row>
     <row r="11" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
@@ -2254,7 +2263,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="5">
         <v>0</v>
@@ -2274,7 +2283,7 @@
     </row>
     <row r="12" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="5">
         <v>1</v>
@@ -2286,7 +2295,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="5">
         <v>0</v>
@@ -2310,7 +2319,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="5">
         <v>0</v>
@@ -2324,7 +2333,7 @@
     </row>
     <row r="13" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -2374,7 +2383,7 @@
     </row>
     <row r="14" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
-        <v>77</v>
+        <v>12</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
@@ -2410,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N14" s="5">
         <v>0</v>
@@ -2424,158 +2433,158 @@
     </row>
     <row r="15" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
+      <c r="I15" s="5">
+        <v>0</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0</v>
+      </c>
+      <c r="L15" s="5">
+        <v>0</v>
+      </c>
+      <c r="M15" s="5">
+        <v>1</v>
+      </c>
+      <c r="N15" s="5">
+        <v>0</v>
+      </c>
+      <c r="O15" s="5">
+        <v>0</v>
+      </c>
+      <c r="P15" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-      <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0</v>
-      </c>
-      <c r="E15" s="5">
-        <v>0</v>
-      </c>
-      <c r="F15" s="5">
-        <v>0</v>
-      </c>
-      <c r="G15" s="5">
-        <v>0</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0</v>
-      </c>
-      <c r="I15" s="5">
-        <v>0</v>
-      </c>
-      <c r="J15" s="5">
-        <v>0</v>
-      </c>
-      <c r="K15" s="5">
-        <v>0</v>
-      </c>
-      <c r="L15" s="5">
-        <v>0</v>
-      </c>
-      <c r="M15" s="5">
-        <v>0</v>
-      </c>
-      <c r="N15" s="5">
-        <v>0</v>
-      </c>
-      <c r="O15" s="5">
-        <v>0</v>
-      </c>
-      <c r="P15" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0</v>
+      </c>
+      <c r="L16" s="5">
+        <v>0</v>
+      </c>
+      <c r="M16" s="5">
+        <v>0</v>
+      </c>
+      <c r="N16" s="5">
+        <v>0</v>
+      </c>
+      <c r="O16" s="5">
+        <v>0</v>
+      </c>
+      <c r="P16" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="5">
-        <v>1</v>
-      </c>
-      <c r="C16" s="5">
-        <v>1</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1</v>
-      </c>
-      <c r="E16" s="5">
-        <v>0</v>
-      </c>
-      <c r="F16" s="5">
-        <v>0</v>
-      </c>
-      <c r="G16" s="5">
-        <v>0</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0</v>
-      </c>
-      <c r="I16" s="5">
-        <v>0</v>
-      </c>
-      <c r="J16" s="5">
-        <v>0</v>
-      </c>
-      <c r="K16" s="5">
-        <v>0</v>
-      </c>
-      <c r="L16" s="5">
-        <v>0</v>
-      </c>
-      <c r="M16" s="5">
-        <v>0</v>
-      </c>
-      <c r="N16" s="5">
-        <v>0</v>
-      </c>
-      <c r="O16" s="5">
-        <v>0</v>
-      </c>
-      <c r="P16" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="4" t="s">
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0</v>
+      </c>
+      <c r="L17" s="5">
+        <v>0</v>
+      </c>
+      <c r="M17" s="5">
+        <v>0</v>
+      </c>
+      <c r="N17" s="5">
+        <v>0</v>
+      </c>
+      <c r="O17" s="5">
+        <v>0</v>
+      </c>
+      <c r="P17" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="5">
-        <v>1</v>
-      </c>
-      <c r="C17" s="5">
-        <v>1</v>
-      </c>
-      <c r="D17" s="5">
-        <v>1</v>
-      </c>
-      <c r="E17" s="5">
-        <v>1</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0</v>
-      </c>
-      <c r="G17" s="5">
-        <v>0</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
-        <v>0</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0</v>
-      </c>
-      <c r="K17" s="5">
-        <v>1</v>
-      </c>
-      <c r="L17" s="5">
-        <v>0</v>
-      </c>
-      <c r="M17" s="5">
-        <v>0</v>
-      </c>
-      <c r="N17" s="5">
-        <v>0</v>
-      </c>
-      <c r="O17" s="5">
-        <v>0</v>
-      </c>
-      <c r="P17" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="B18" s="5">
         <v>1</v>
       </c>
@@ -2610,7 +2619,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" s="5">
         <v>0</v>
@@ -2624,7 +2633,7 @@
     </row>
     <row r="19" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
       <c r="B19" s="5">
         <v>1</v>
@@ -2636,7 +2645,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="5">
         <v>0</v>
@@ -2654,7 +2663,7 @@
         <v>0</v>
       </c>
       <c r="K19" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="5">
         <v>0</v>
@@ -2674,7 +2683,7 @@
     </row>
     <row r="20" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
@@ -2686,7 +2695,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="5">
         <v>0</v>
@@ -2710,7 +2719,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20" s="5">
         <v>0</v>
@@ -2724,58 +2733,58 @@
     </row>
     <row r="21" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5">
+        <v>1</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <v>0</v>
+      </c>
+      <c r="K21" s="5">
+        <v>0</v>
+      </c>
+      <c r="L21" s="5">
+        <v>0</v>
+      </c>
+      <c r="M21" s="5">
+        <v>0</v>
+      </c>
+      <c r="N21" s="5">
+        <v>0</v>
+      </c>
+      <c r="O21" s="5">
+        <v>0</v>
+      </c>
+      <c r="P21" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="5">
-        <v>1</v>
-      </c>
-      <c r="C21" s="5">
-        <v>1</v>
-      </c>
-      <c r="D21" s="5">
-        <v>1</v>
-      </c>
-      <c r="E21" s="5">
-        <v>1</v>
-      </c>
-      <c r="F21" s="5">
-        <v>0</v>
-      </c>
-      <c r="G21" s="5">
-        <v>0</v>
-      </c>
-      <c r="H21" s="5">
-        <v>0</v>
-      </c>
-      <c r="I21" s="5">
-        <v>0</v>
-      </c>
-      <c r="J21" s="5">
-        <v>0</v>
-      </c>
-      <c r="K21" s="5">
-        <v>0</v>
-      </c>
-      <c r="L21" s="5">
-        <v>0</v>
-      </c>
-      <c r="M21" s="5">
-        <v>1</v>
-      </c>
-      <c r="N21" s="5">
-        <v>0</v>
-      </c>
-      <c r="O21" s="5">
-        <v>0</v>
-      </c>
-      <c r="P21" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="B22" s="5">
         <v>1</v>
       </c>
@@ -2783,7 +2792,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
@@ -2810,7 +2819,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="5">
         <v>0</v>
@@ -2824,66 +2833,66 @@
     </row>
     <row r="23" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5">
+        <v>0</v>
+      </c>
+      <c r="E23" s="5">
+        <v>1</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0</v>
+      </c>
+      <c r="J23" s="5">
+        <v>0</v>
+      </c>
+      <c r="K23" s="5">
+        <v>0</v>
+      </c>
+      <c r="L23" s="5">
+        <v>0</v>
+      </c>
+      <c r="M23" s="5">
+        <v>0</v>
+      </c>
+      <c r="N23" s="5">
+        <v>0</v>
+      </c>
+      <c r="O23" s="5">
+        <v>0</v>
+      </c>
+      <c r="P23" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B23" s="5">
-        <v>1</v>
-      </c>
-      <c r="C23" s="5">
-        <v>1</v>
-      </c>
-      <c r="D23" s="5">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5">
-        <v>0</v>
-      </c>
-      <c r="F23" s="5">
-        <v>0</v>
-      </c>
-      <c r="G23" s="5">
-        <v>0</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0</v>
-      </c>
-      <c r="I23" s="5">
-        <v>0</v>
-      </c>
-      <c r="J23" s="5">
-        <v>0</v>
-      </c>
-      <c r="K23" s="5">
-        <v>1</v>
-      </c>
-      <c r="L23" s="5">
-        <v>0</v>
-      </c>
-      <c r="M23" s="5">
-        <v>0</v>
-      </c>
-      <c r="N23" s="5">
-        <v>0</v>
-      </c>
-      <c r="O23" s="5">
-        <v>0</v>
-      </c>
-      <c r="P23" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="B24" s="5">
         <v>1</v>
       </c>
       <c r="C24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="5">
         <v>0</v>
@@ -2904,7 +2913,7 @@
         <v>0</v>
       </c>
       <c r="K24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" s="5">
         <v>0</v>
@@ -2924,10 +2933,10 @@
     </row>
     <row r="25" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="B25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="5">
         <v>0</v>
@@ -2969,12 +2978,12 @@
         <v>0</v>
       </c>
       <c r="P25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" s="5">
         <v>0</v>
@@ -3024,57 +3033,57 @@
     </row>
     <row r="27" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="5">
+        <v>0</v>
+      </c>
+      <c r="C27" s="5">
+        <v>0</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0</v>
+      </c>
+      <c r="E27" s="5">
+        <v>0</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
+        <v>0</v>
+      </c>
+      <c r="J27" s="5">
+        <v>0</v>
+      </c>
+      <c r="K27" s="5">
+        <v>0</v>
+      </c>
+      <c r="L27" s="5">
+        <v>0</v>
+      </c>
+      <c r="M27" s="5">
+        <v>0</v>
+      </c>
+      <c r="N27" s="5">
+        <v>0</v>
+      </c>
+      <c r="O27" s="5">
+        <v>0</v>
+      </c>
+      <c r="P27" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B27" s="5">
-        <v>0</v>
-      </c>
-      <c r="C27" s="5">
-        <v>0</v>
-      </c>
-      <c r="D27" s="5">
-        <v>0</v>
-      </c>
-      <c r="E27" s="5">
-        <v>0</v>
-      </c>
-      <c r="F27" s="5">
-        <v>0</v>
-      </c>
-      <c r="G27" s="5">
-        <v>0</v>
-      </c>
-      <c r="H27" s="5">
-        <v>0</v>
-      </c>
-      <c r="I27" s="5">
-        <v>0</v>
-      </c>
-      <c r="J27" s="5">
-        <v>0</v>
-      </c>
-      <c r="K27" s="5">
-        <v>1</v>
-      </c>
-      <c r="L27" s="5">
-        <v>0</v>
-      </c>
-      <c r="M27" s="5">
-        <v>0</v>
-      </c>
-      <c r="N27" s="5">
-        <v>0</v>
-      </c>
-      <c r="O27" s="5">
-        <v>0</v>
-      </c>
-      <c r="P27" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="B28" s="5">
         <v>0</v>
@@ -3124,58 +3133,58 @@
     </row>
     <row r="29" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="5">
+        <v>0</v>
+      </c>
+      <c r="C29" s="5">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <v>0</v>
+      </c>
+      <c r="J29" s="5">
+        <v>0</v>
+      </c>
+      <c r="K29" s="5">
+        <v>1</v>
+      </c>
+      <c r="L29" s="5">
+        <v>0</v>
+      </c>
+      <c r="M29" s="5">
+        <v>0</v>
+      </c>
+      <c r="N29" s="5">
+        <v>0</v>
+      </c>
+      <c r="O29" s="5">
+        <v>0</v>
+      </c>
+      <c r="P29" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B29" s="5">
-        <v>0</v>
-      </c>
-      <c r="C29" s="5">
-        <v>0</v>
-      </c>
-      <c r="D29" s="5">
-        <v>0</v>
-      </c>
-      <c r="E29" s="5">
-        <v>0</v>
-      </c>
-      <c r="F29" s="5">
-        <v>0</v>
-      </c>
-      <c r="G29" s="5">
-        <v>0</v>
-      </c>
-      <c r="H29" s="5">
-        <v>0</v>
-      </c>
-      <c r="I29" s="5">
-        <v>0</v>
-      </c>
-      <c r="J29" s="5">
-        <v>0</v>
-      </c>
-      <c r="K29" s="5">
-        <v>1</v>
-      </c>
-      <c r="L29" s="5">
-        <v>0</v>
-      </c>
-      <c r="M29" s="5">
-        <v>0</v>
-      </c>
-      <c r="N29" s="5">
-        <v>0</v>
-      </c>
-      <c r="O29" s="5">
-        <v>0</v>
-      </c>
-      <c r="P29" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="B30" s="5">
         <v>0</v>
       </c>
@@ -3204,7 +3213,7 @@
         <v>0</v>
       </c>
       <c r="K30" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L30" s="5">
         <v>0</v>
@@ -3224,7 +3233,7 @@
     </row>
     <row r="31" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B31" s="5">
         <v>0</v>
@@ -3274,7 +3283,7 @@
     </row>
     <row r="32" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="B32" s="5">
         <v>0</v>
@@ -3324,7 +3333,7 @@
     </row>
     <row r="33" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B33" s="5">
         <v>0</v>
@@ -3354,7 +3363,7 @@
         <v>0</v>
       </c>
       <c r="K33" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L33" s="5">
         <v>0</v>
@@ -3369,62 +3378,62 @@
         <v>0</v>
       </c>
       <c r="P33" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="5">
+        <v>0</v>
+      </c>
+      <c r="C34" s="5">
+        <v>0</v>
+      </c>
+      <c r="D34" s="5">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5">
+        <v>0</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0</v>
+      </c>
+      <c r="I34" s="5">
+        <v>0</v>
+      </c>
+      <c r="J34" s="5">
+        <v>0</v>
+      </c>
+      <c r="K34" s="5">
+        <v>1</v>
+      </c>
+      <c r="L34" s="5">
+        <v>0</v>
+      </c>
+      <c r="M34" s="5">
+        <v>0</v>
+      </c>
+      <c r="N34" s="5">
+        <v>0</v>
+      </c>
+      <c r="O34" s="5">
+        <v>0</v>
+      </c>
+      <c r="P34" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A35" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="B34" s="5">
-        <v>0</v>
-      </c>
-      <c r="C34" s="5">
-        <v>0</v>
-      </c>
-      <c r="D34" s="5">
-        <v>0</v>
-      </c>
-      <c r="E34" s="5">
-        <v>0</v>
-      </c>
-      <c r="F34" s="5">
-        <v>0</v>
-      </c>
-      <c r="G34" s="5">
-        <v>0</v>
-      </c>
-      <c r="H34" s="5">
-        <v>0</v>
-      </c>
-      <c r="I34" s="5">
-        <v>0</v>
-      </c>
-      <c r="J34" s="5">
-        <v>0</v>
-      </c>
-      <c r="K34" s="5">
-        <v>1</v>
-      </c>
-      <c r="L34" s="5">
-        <v>0</v>
-      </c>
-      <c r="M34" s="5">
-        <v>0</v>
-      </c>
-      <c r="N34" s="5">
-        <v>0</v>
-      </c>
-      <c r="O34" s="5">
-        <v>0</v>
-      </c>
-      <c r="P34" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="B35" s="5">
         <v>0</v>
@@ -3474,58 +3483,58 @@
     </row>
     <row r="36" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0</v>
+      </c>
+      <c r="D36" s="5">
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <v>0</v>
+      </c>
+      <c r="F36" s="5">
+        <v>0</v>
+      </c>
+      <c r="G36" s="5">
+        <v>0</v>
+      </c>
+      <c r="H36" s="5">
+        <v>0</v>
+      </c>
+      <c r="I36" s="5">
+        <v>0</v>
+      </c>
+      <c r="J36" s="5">
+        <v>0</v>
+      </c>
+      <c r="K36" s="5">
+        <v>1</v>
+      </c>
+      <c r="L36" s="5">
+        <v>0</v>
+      </c>
+      <c r="M36" s="5">
+        <v>0</v>
+      </c>
+      <c r="N36" s="5">
+        <v>0</v>
+      </c>
+      <c r="O36" s="5">
+        <v>0</v>
+      </c>
+      <c r="P36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A37" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="5">
-        <v>0</v>
-      </c>
-      <c r="C36" s="5">
-        <v>0</v>
-      </c>
-      <c r="D36" s="5">
-        <v>0</v>
-      </c>
-      <c r="E36" s="5">
-        <v>0</v>
-      </c>
-      <c r="F36" s="5">
-        <v>0</v>
-      </c>
-      <c r="G36" s="5">
-        <v>0</v>
-      </c>
-      <c r="H36" s="5">
-        <v>0</v>
-      </c>
-      <c r="I36" s="5">
-        <v>0</v>
-      </c>
-      <c r="J36" s="5">
-        <v>0</v>
-      </c>
-      <c r="K36" s="5">
-        <v>1</v>
-      </c>
-      <c r="L36" s="5">
-        <v>0</v>
-      </c>
-      <c r="M36" s="5">
-        <v>0</v>
-      </c>
-      <c r="N36" s="5">
-        <v>0</v>
-      </c>
-      <c r="O36" s="5">
-        <v>0</v>
-      </c>
-      <c r="P36" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="B37" s="5">
         <v>0</v>
       </c>
@@ -3554,13 +3563,13 @@
         <v>0</v>
       </c>
       <c r="K37" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L37" s="5">
         <v>0</v>
       </c>
       <c r="M37" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N37" s="5">
         <v>0</v>
@@ -3574,7 +3583,7 @@
     </row>
     <row r="38" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B38" s="5">
         <v>0</v>
@@ -3607,10 +3616,10 @@
         <v>0</v>
       </c>
       <c r="L38" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M38" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N38" s="5">
         <v>0</v>
@@ -3624,7 +3633,7 @@
     </row>
     <row r="39" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
       <c r="B39" s="5">
         <v>0</v>
@@ -3654,13 +3663,13 @@
         <v>0</v>
       </c>
       <c r="K39" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L39" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N39" s="5">
         <v>0</v>
@@ -3674,7 +3683,7 @@
     </row>
     <row r="40" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B40" s="5">
         <v>0</v>
@@ -3724,208 +3733,208 @@
     </row>
     <row r="41" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="5">
+        <v>0</v>
+      </c>
+      <c r="C41" s="5">
+        <v>0</v>
+      </c>
+      <c r="D41" s="5">
+        <v>0</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0</v>
+      </c>
+      <c r="H41" s="5">
+        <v>0</v>
+      </c>
+      <c r="I41" s="5">
+        <v>0</v>
+      </c>
+      <c r="J41" s="5">
+        <v>0</v>
+      </c>
+      <c r="K41" s="5">
+        <v>0</v>
+      </c>
+      <c r="L41" s="5">
+        <v>1</v>
+      </c>
+      <c r="M41" s="5">
+        <v>0</v>
+      </c>
+      <c r="N41" s="5">
+        <v>0</v>
+      </c>
+      <c r="O41" s="5">
+        <v>0</v>
+      </c>
+      <c r="P41" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="5">
+        <v>0</v>
+      </c>
+      <c r="C42" s="5">
+        <v>0</v>
+      </c>
+      <c r="D42" s="5">
+        <v>0</v>
+      </c>
+      <c r="E42" s="5">
+        <v>0</v>
+      </c>
+      <c r="F42" s="5">
+        <v>0</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0</v>
+      </c>
+      <c r="I42" s="5">
+        <v>0</v>
+      </c>
+      <c r="J42" s="5">
+        <v>0</v>
+      </c>
+      <c r="K42" s="5">
+        <v>0</v>
+      </c>
+      <c r="L42" s="5">
+        <v>1</v>
+      </c>
+      <c r="M42" s="5">
+        <v>0</v>
+      </c>
+      <c r="N42" s="5">
+        <v>0</v>
+      </c>
+      <c r="O42" s="5">
+        <v>0</v>
+      </c>
+      <c r="P42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A43" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B41" s="5">
-        <v>0</v>
-      </c>
-      <c r="C41" s="5">
-        <v>0</v>
-      </c>
-      <c r="D41" s="5">
-        <v>0</v>
-      </c>
-      <c r="E41" s="5">
-        <v>0</v>
-      </c>
-      <c r="F41" s="5">
-        <v>0</v>
-      </c>
-      <c r="G41" s="5">
-        <v>0</v>
-      </c>
-      <c r="H41" s="5">
-        <v>0</v>
-      </c>
-      <c r="I41" s="5">
-        <v>0</v>
-      </c>
-      <c r="J41" s="5">
-        <v>0</v>
-      </c>
-      <c r="K41" s="5">
-        <v>0</v>
-      </c>
-      <c r="L41" s="5">
-        <v>1</v>
-      </c>
-      <c r="M41" s="5">
-        <v>0</v>
-      </c>
-      <c r="N41" s="5">
-        <v>0</v>
-      </c>
-      <c r="O41" s="5">
-        <v>0</v>
-      </c>
-      <c r="P41" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+      <c r="B43" s="5">
+        <v>0</v>
+      </c>
+      <c r="C43" s="5">
+        <v>0</v>
+      </c>
+      <c r="D43" s="5">
+        <v>0</v>
+      </c>
+      <c r="E43" s="5">
+        <v>0</v>
+      </c>
+      <c r="F43" s="5">
+        <v>0</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0</v>
+      </c>
+      <c r="I43" s="5">
+        <v>0</v>
+      </c>
+      <c r="J43" s="5">
+        <v>0</v>
+      </c>
+      <c r="K43" s="5">
+        <v>0</v>
+      </c>
+      <c r="L43" s="5">
+        <v>1</v>
+      </c>
+      <c r="M43" s="5">
+        <v>0</v>
+      </c>
+      <c r="N43" s="5">
+        <v>0</v>
+      </c>
+      <c r="O43" s="5">
+        <v>0</v>
+      </c>
+      <c r="P43" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
         <v>98</v>
       </c>
-      <c r="B42" s="5">
-        <v>0</v>
-      </c>
-      <c r="C42" s="5">
-        <v>0</v>
-      </c>
-      <c r="D42" s="5">
-        <v>0</v>
-      </c>
-      <c r="E42" s="5">
-        <v>0</v>
-      </c>
-      <c r="F42" s="5">
-        <v>0</v>
-      </c>
-      <c r="G42" s="5">
-        <v>0</v>
-      </c>
-      <c r="H42" s="5">
-        <v>0</v>
-      </c>
-      <c r="I42" s="5">
-        <v>0</v>
-      </c>
-      <c r="J42" s="5">
-        <v>0</v>
-      </c>
-      <c r="K42" s="5">
-        <v>0</v>
-      </c>
-      <c r="L42" s="5">
-        <v>0</v>
-      </c>
-      <c r="M42" s="5">
-        <v>0</v>
-      </c>
-      <c r="N42" s="5">
-        <v>0</v>
-      </c>
-      <c r="O42" s="5">
-        <v>0</v>
-      </c>
-      <c r="P42" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+      <c r="B44" s="5">
+        <v>0</v>
+      </c>
+      <c r="C44" s="5">
+        <v>0</v>
+      </c>
+      <c r="D44" s="5">
+        <v>0</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0</v>
+      </c>
+      <c r="F44" s="5">
+        <v>0</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0</v>
+      </c>
+      <c r="I44" s="5">
+        <v>0</v>
+      </c>
+      <c r="J44" s="5">
+        <v>0</v>
+      </c>
+      <c r="K44" s="5">
+        <v>0</v>
+      </c>
+      <c r="L44" s="5">
+        <v>0</v>
+      </c>
+      <c r="M44" s="5">
+        <v>0</v>
+      </c>
+      <c r="N44" s="5">
+        <v>0</v>
+      </c>
+      <c r="O44" s="5">
+        <v>0</v>
+      </c>
+      <c r="P44" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>99</v>
       </c>
-      <c r="B43" s="5">
-        <v>0</v>
-      </c>
-      <c r="C43" s="5">
-        <v>0</v>
-      </c>
-      <c r="D43" s="5">
-        <v>0</v>
-      </c>
-      <c r="E43" s="5">
-        <v>0</v>
-      </c>
-      <c r="F43" s="5">
-        <v>0</v>
-      </c>
-      <c r="G43" s="5">
-        <v>0</v>
-      </c>
-      <c r="H43" s="5">
-        <v>0</v>
-      </c>
-      <c r="I43" s="5">
-        <v>0</v>
-      </c>
-      <c r="J43" s="5">
-        <v>0</v>
-      </c>
-      <c r="K43" s="5">
-        <v>0</v>
-      </c>
-      <c r="L43" s="5">
-        <v>0</v>
-      </c>
-      <c r="M43" s="5">
-        <v>0</v>
-      </c>
-      <c r="N43" s="5">
-        <v>0</v>
-      </c>
-      <c r="O43" s="5">
-        <v>0</v>
-      </c>
-      <c r="P43" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B44" s="5">
-        <v>0</v>
-      </c>
-      <c r="C44" s="5">
-        <v>0</v>
-      </c>
-      <c r="D44" s="5">
-        <v>0</v>
-      </c>
-      <c r="E44" s="5">
-        <v>0</v>
-      </c>
-      <c r="F44" s="5">
-        <v>0</v>
-      </c>
-      <c r="G44" s="5">
-        <v>0</v>
-      </c>
-      <c r="H44" s="5">
-        <v>0</v>
-      </c>
-      <c r="I44" s="5">
-        <v>0</v>
-      </c>
-      <c r="J44" s="5">
-        <v>0</v>
-      </c>
-      <c r="K44" s="5">
-        <v>0</v>
-      </c>
-      <c r="L44" s="5">
-        <v>0</v>
-      </c>
-      <c r="M44" s="5">
-        <v>0</v>
-      </c>
-      <c r="N44" s="5">
-        <v>0</v>
-      </c>
-      <c r="O44" s="5">
-        <v>0</v>
-      </c>
-      <c r="P44" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="B45" s="5">
         <v>0</v>
       </c>
@@ -3936,7 +3945,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F45" s="5">
         <v>0</v>
@@ -3969,12 +3978,12 @@
         <v>0</v>
       </c>
       <c r="P45" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="1" t="s">
-        <v>19</v>
+      <c r="A46" t="s">
+        <v>114</v>
       </c>
       <c r="B46" s="5">
         <v>0</v>
@@ -4024,7 +4033,7 @@
     </row>
     <row r="47" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>20</v>
+        <v>97</v>
       </c>
       <c r="B47" s="5">
         <v>0</v>
@@ -4074,7 +4083,7 @@
     </row>
     <row r="48" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B48" s="5">
         <v>0</v>
@@ -4086,10 +4095,10 @@
         <v>0</v>
       </c>
       <c r="E48" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F48" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G48" s="5">
         <v>0</v>
@@ -4124,7 +4133,7 @@
     </row>
     <row r="49" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>109</v>
+        <v>19</v>
       </c>
       <c r="B49" s="5">
         <v>0</v>
@@ -4148,7 +4157,7 @@
         <v>0</v>
       </c>
       <c r="I49" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" s="5">
         <v>0</v>
@@ -4169,12 +4178,12 @@
         <v>0</v>
       </c>
       <c r="P49" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B50" s="5">
         <v>0</v>
@@ -4198,7 +4207,7 @@
         <v>0</v>
       </c>
       <c r="I50" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J50" s="5">
         <v>0</v>
@@ -4219,12 +4228,12 @@
         <v>0</v>
       </c>
       <c r="P50" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B51" s="5">
         <v>0</v>
@@ -4239,7 +4248,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="5">
         <v>0</v>
@@ -4248,7 +4257,7 @@
         <v>0</v>
       </c>
       <c r="I51" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J51" s="5">
         <v>0</v>
@@ -4274,7 +4283,7 @@
     </row>
     <row r="52" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B52" s="5">
         <v>0</v>
@@ -4324,7 +4333,7 @@
     </row>
     <row r="53" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B53" s="5">
         <v>0</v>
@@ -4374,7 +4383,7 @@
     </row>
     <row r="54" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B54" s="5">
         <v>0</v>
@@ -4424,7 +4433,7 @@
     </row>
     <row r="55" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="B55" s="5">
         <v>0</v>
@@ -4474,7 +4483,7 @@
     </row>
     <row r="56" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B56" s="5">
         <v>0</v>
@@ -4510,7 +4519,7 @@
         <v>0</v>
       </c>
       <c r="M56" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N56" s="5">
         <v>0</v>
@@ -4524,7 +4533,7 @@
     </row>
     <row r="57" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="B57" s="5">
         <v>0</v>
@@ -4574,7 +4583,7 @@
     </row>
     <row r="58" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>110</v>
+        <v>46</v>
       </c>
       <c r="B58" s="5">
         <v>0</v>
@@ -4624,7 +4633,7 @@
     </row>
     <row r="59" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="B59" s="5">
         <v>0</v>
@@ -4660,7 +4669,7 @@
         <v>0</v>
       </c>
       <c r="M59" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N59" s="5">
         <v>0</v>
@@ -4674,7 +4683,7 @@
     </row>
     <row r="60" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B60" s="5">
         <v>0</v>
@@ -4724,7 +4733,7 @@
     </row>
     <row r="61" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B61" s="5">
         <v>0</v>
@@ -4774,7 +4783,7 @@
     </row>
     <row r="62" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="B62" s="5">
         <v>0</v>
@@ -4823,8 +4832,8 @@
       </c>
     </row>
     <row r="63" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A63" s="4" t="s">
-        <v>22</v>
+      <c r="A63" s="1" t="s">
+        <v>108</v>
       </c>
       <c r="B63" s="5">
         <v>0</v>
@@ -4839,16 +4848,16 @@
         <v>0</v>
       </c>
       <c r="F63" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G63" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H63" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J63" s="5">
         <v>0</v>
@@ -4874,7 +4883,7 @@
     </row>
     <row r="64" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="B64" s="5">
         <v>0</v>
@@ -4889,19 +4898,19 @@
         <v>0</v>
       </c>
       <c r="F64" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G64" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H64" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J64" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K64" s="5">
         <v>0</v>
@@ -4924,7 +4933,7 @@
     </row>
     <row r="65" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="B65" s="5">
         <v>0</v>
@@ -4939,16 +4948,16 @@
         <v>0</v>
       </c>
       <c r="F65" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G65" s="5">
         <v>0</v>
       </c>
       <c r="H65" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J65" s="5">
         <v>0</v>
@@ -4973,8 +4982,8 @@
       </c>
     </row>
     <row r="66" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A66" s="1" t="s">
-        <v>49</v>
+      <c r="A66" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B66" s="5">
         <v>0</v>
@@ -4989,13 +4998,13 @@
         <v>0</v>
       </c>
       <c r="F66" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66" s="5">
         <v>1</v>
       </c>
       <c r="H66" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66" s="5">
         <v>0</v>
@@ -5024,7 +5033,7 @@
     </row>
     <row r="67" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="B67" s="5">
         <v>0</v>
@@ -5036,22 +5045,22 @@
         <v>0</v>
       </c>
       <c r="E67" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F67" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I67" s="5">
         <v>0</v>
       </c>
       <c r="J67" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K67" s="5">
         <v>0</v>
@@ -5074,7 +5083,7 @@
     </row>
     <row r="68" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>103</v>
+        <v>23</v>
       </c>
       <c r="B68" s="5">
         <v>0</v>
@@ -5083,19 +5092,19 @@
         <v>0</v>
       </c>
       <c r="D68" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68" s="5">
         <v>0</v>
       </c>
       <c r="F68" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G68" s="5">
         <v>0</v>
       </c>
       <c r="H68" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68" s="5">
         <v>0</v>
@@ -5124,7 +5133,7 @@
     </row>
     <row r="69" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B69" s="5">
         <v>0</v>
@@ -5142,7 +5151,7 @@
         <v>0</v>
       </c>
       <c r="G69" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H69" s="5">
         <v>0</v>
@@ -5163,7 +5172,7 @@
         <v>0</v>
       </c>
       <c r="N69" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O69" s="5">
         <v>0</v>
@@ -5174,7 +5183,7 @@
     </row>
     <row r="70" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B70" s="5">
         <v>0</v>
@@ -5186,7 +5195,7 @@
         <v>0</v>
       </c>
       <c r="E70" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F70" s="5">
         <v>0</v>
@@ -5213,7 +5222,7 @@
         <v>0</v>
       </c>
       <c r="N70" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O70" s="5">
         <v>0</v>
@@ -5224,7 +5233,7 @@
     </row>
     <row r="71" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="B71" s="5">
         <v>0</v>
@@ -5233,7 +5242,7 @@
         <v>0</v>
       </c>
       <c r="D71" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71" s="5">
         <v>0</v>
@@ -5263,7 +5272,7 @@
         <v>0</v>
       </c>
       <c r="N71" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O71" s="5">
         <v>0</v>
@@ -5274,7 +5283,7 @@
     </row>
     <row r="72" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B72" s="5">
         <v>0</v>
@@ -5324,7 +5333,7 @@
     </row>
     <row r="73" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B73" s="5">
         <v>0</v>
@@ -5374,7 +5383,7 @@
     </row>
     <row r="74" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="B74" s="5">
         <v>0</v>
@@ -5424,7 +5433,7 @@
     </row>
     <row r="75" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B75" s="5">
         <v>0</v>
@@ -5474,7 +5483,7 @@
     </row>
     <row r="76" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="B76" s="5">
         <v>0</v>
@@ -5524,7 +5533,7 @@
     </row>
     <row r="77" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B77" s="5">
         <v>0</v>
@@ -5574,7 +5583,7 @@
     </row>
     <row r="78" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="B78" s="5">
         <v>0</v>
@@ -5586,7 +5595,7 @@
         <v>0</v>
       </c>
       <c r="E78" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F78" s="5">
         <v>0</v>
@@ -5613,7 +5622,7 @@
         <v>0</v>
       </c>
       <c r="N78" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O78" s="5">
         <v>0</v>
@@ -5624,7 +5633,7 @@
     </row>
     <row r="79" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="B79" s="5">
         <v>0</v>
@@ -5645,7 +5654,7 @@
         <v>0</v>
       </c>
       <c r="H79" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I79" s="5">
         <v>0</v>
@@ -5663,7 +5672,7 @@
         <v>0</v>
       </c>
       <c r="N79" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O79" s="5">
         <v>0</v>
@@ -5674,7 +5683,7 @@
     </row>
     <row r="80" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="B80" s="5">
         <v>0</v>
@@ -5713,18 +5722,18 @@
         <v>0</v>
       </c>
       <c r="N80" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O80" s="5">
         <v>0</v>
       </c>
       <c r="P80" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="B81" s="5">
         <v>0</v>
@@ -5736,7 +5745,7 @@
         <v>0</v>
       </c>
       <c r="E81" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81" s="5">
         <v>0</v>
@@ -5766,7 +5775,7 @@
         <v>0</v>
       </c>
       <c r="O81" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P81" s="5">
         <v>0</v>
@@ -5774,7 +5783,7 @@
     </row>
     <row r="82" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
-        <v>57</v>
+        <v>25</v>
       </c>
       <c r="B82" s="5">
         <v>0</v>
@@ -5795,7 +5804,7 @@
         <v>0</v>
       </c>
       <c r="H82" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I82" s="5">
         <v>0</v>
@@ -5816,7 +5825,7 @@
         <v>0</v>
       </c>
       <c r="O82" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P82" s="5">
         <v>0</v>
@@ -5824,7 +5833,7 @@
     </row>
     <row r="83" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="B83" s="5">
         <v>0</v>
@@ -5866,15 +5875,15 @@
         <v>0</v>
       </c>
       <c r="O83" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P83" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A84" s="4" t="s">
-        <v>82</v>
+      <c r="A84" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="B84" s="5">
         <v>0</v>
@@ -5916,15 +5925,15 @@
         <v>0</v>
       </c>
       <c r="O84" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P84" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B85" s="5">
         <v>0</v>
@@ -5966,21 +5975,21 @@
         <v>0</v>
       </c>
       <c r="O85" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P85" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="B86" s="5">
         <v>0</v>
       </c>
       <c r="C86" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" s="5">
         <v>0</v>
@@ -6016,15 +6025,15 @@
         <v>0</v>
       </c>
       <c r="O86" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P86" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A87" s="1" t="s">
-        <v>27</v>
+      <c r="A87" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="B87" s="5">
         <v>0</v>
@@ -6074,13 +6083,13 @@
     </row>
     <row r="88" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="B88" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C88" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D88" s="5">
         <v>0</v>
@@ -6119,21 +6128,21 @@
         <v>0</v>
       </c>
       <c r="P88" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="B89" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C89" s="5">
         <v>1</v>
       </c>
       <c r="D89" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89" s="5">
         <v>0</v>
@@ -6174,19 +6183,19 @@
     </row>
     <row r="90" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="B90" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C90" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D90" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F90" s="5">
         <v>0</v>
@@ -6219,12 +6228,12 @@
         <v>0</v>
       </c>
       <c r="P90" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B91" s="5">
         <v>1</v>
@@ -6236,7 +6245,7 @@
         <v>0</v>
       </c>
       <c r="E91" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F91" s="5">
         <v>0</v>
@@ -6274,16 +6283,16 @@
     </row>
     <row r="92" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B92" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C92" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D92" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92" s="5">
         <v>0</v>
@@ -6319,24 +6328,24 @@
         <v>0</v>
       </c>
       <c r="P92" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B93" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C93" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D93" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E93" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F93" s="5">
         <v>0</v>
@@ -6369,24 +6378,24 @@
         <v>0</v>
       </c>
       <c r="P93" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="B94" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C94" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D94" s="5">
         <v>0</v>
       </c>
       <c r="E94" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F94" s="5">
         <v>0</v>
@@ -6419,12 +6428,12 @@
         <v>0</v>
       </c>
       <c r="P94" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B95" s="5">
         <v>0</v>
@@ -6451,7 +6460,7 @@
         <v>0</v>
       </c>
       <c r="J95" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K95" s="5">
         <v>0</v>
@@ -6469,12 +6478,12 @@
         <v>0</v>
       </c>
       <c r="P95" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="B96" s="5">
         <v>0</v>
@@ -6524,7 +6533,7 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="B97" s="5">
         <v>0</v>
@@ -6574,57 +6583,207 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B98" s="5">
+        <v>0</v>
+      </c>
+      <c r="C98" s="5">
+        <v>0</v>
+      </c>
+      <c r="D98" s="5">
+        <v>0</v>
+      </c>
+      <c r="E98" s="5">
+        <v>0</v>
+      </c>
+      <c r="F98" s="5">
+        <v>0</v>
+      </c>
+      <c r="G98" s="5">
+        <v>0</v>
+      </c>
+      <c r="H98" s="5">
+        <v>0</v>
+      </c>
+      <c r="I98" s="5">
+        <v>0</v>
+      </c>
+      <c r="J98" s="5">
+        <v>1</v>
+      </c>
+      <c r="K98" s="5">
+        <v>0</v>
+      </c>
+      <c r="L98" s="5">
+        <v>0</v>
+      </c>
+      <c r="M98" s="5">
+        <v>0</v>
+      </c>
+      <c r="N98" s="5">
+        <v>0</v>
+      </c>
+      <c r="O98" s="5">
+        <v>0</v>
+      </c>
+      <c r="P98" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A99" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B99" s="5">
+        <v>0</v>
+      </c>
+      <c r="C99" s="5">
+        <v>0</v>
+      </c>
+      <c r="D99" s="5">
+        <v>0</v>
+      </c>
+      <c r="E99" s="5">
+        <v>0</v>
+      </c>
+      <c r="F99" s="5">
+        <v>0</v>
+      </c>
+      <c r="G99" s="5">
+        <v>0</v>
+      </c>
+      <c r="H99" s="5">
+        <v>0</v>
+      </c>
+      <c r="I99" s="5">
+        <v>0</v>
+      </c>
+      <c r="J99" s="5">
+        <v>0</v>
+      </c>
+      <c r="K99" s="5">
+        <v>0</v>
+      </c>
+      <c r="L99" s="5">
+        <v>0</v>
+      </c>
+      <c r="M99" s="5">
+        <v>0</v>
+      </c>
+      <c r="N99" s="5">
+        <v>0</v>
+      </c>
+      <c r="O99" s="5">
+        <v>0</v>
+      </c>
+      <c r="P99" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A100" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B100" s="5">
+        <v>0</v>
+      </c>
+      <c r="C100" s="5">
+        <v>0</v>
+      </c>
+      <c r="D100" s="5">
+        <v>0</v>
+      </c>
+      <c r="E100" s="5">
+        <v>0</v>
+      </c>
+      <c r="F100" s="5">
+        <v>0</v>
+      </c>
+      <c r="G100" s="5">
+        <v>0</v>
+      </c>
+      <c r="H100" s="5">
+        <v>0</v>
+      </c>
+      <c r="I100" s="5">
+        <v>0</v>
+      </c>
+      <c r="J100" s="5">
+        <v>0</v>
+      </c>
+      <c r="K100" s="5">
+        <v>0</v>
+      </c>
+      <c r="L100" s="5">
+        <v>0</v>
+      </c>
+      <c r="M100" s="5">
+        <v>0</v>
+      </c>
+      <c r="N100" s="5">
+        <v>0</v>
+      </c>
+      <c r="O100" s="5">
+        <v>0</v>
+      </c>
+      <c r="P100" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="A101" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B98" s="5">
-        <v>0</v>
-      </c>
-      <c r="C98" s="5">
-        <v>0</v>
-      </c>
-      <c r="D98" s="5">
-        <v>0</v>
-      </c>
-      <c r="E98" s="5">
-        <v>0</v>
-      </c>
-      <c r="F98" s="5">
-        <v>0</v>
-      </c>
-      <c r="G98" s="5">
-        <v>0</v>
-      </c>
-      <c r="H98" s="5">
-        <v>0</v>
-      </c>
-      <c r="I98" s="5">
-        <v>0</v>
-      </c>
-      <c r="J98" s="5">
-        <v>0</v>
-      </c>
-      <c r="K98" s="5">
-        <v>0</v>
-      </c>
-      <c r="L98" s="5">
-        <v>0</v>
-      </c>
-      <c r="M98" s="5">
-        <v>0</v>
-      </c>
-      <c r="N98" s="5">
-        <v>0</v>
-      </c>
-      <c r="O98" s="5">
-        <v>0</v>
-      </c>
-      <c r="P98" s="5">
+      <c r="B101" s="5">
+        <v>0</v>
+      </c>
+      <c r="C101" s="5">
+        <v>0</v>
+      </c>
+      <c r="D101" s="5">
+        <v>0</v>
+      </c>
+      <c r="E101" s="5">
+        <v>0</v>
+      </c>
+      <c r="F101" s="5">
+        <v>0</v>
+      </c>
+      <c r="G101" s="5">
+        <v>0</v>
+      </c>
+      <c r="H101" s="5">
+        <v>0</v>
+      </c>
+      <c r="I101" s="5">
+        <v>0</v>
+      </c>
+      <c r="J101" s="5">
+        <v>0</v>
+      </c>
+      <c r="K101" s="5">
+        <v>0</v>
+      </c>
+      <c r="L101" s="5">
+        <v>0</v>
+      </c>
+      <c r="M101" s="5">
+        <v>0</v>
+      </c>
+      <c r="N101" s="5">
+        <v>0</v>
+      </c>
+      <c r="O101" s="5">
+        <v>0</v>
+      </c>
+      <c r="P101" s="5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:P98">
-    <cfRule type="iconSet" priority="5">
+  <conditionalFormatting sqref="B2:P101">
+    <cfRule type="iconSet" priority="8">
       <iconSet iconSet="5Quarters">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>

</xml_diff>